<commit_message>
Update ICS years, add max account  line
</commit_message>
<xml_diff>
--- a/ICS/IntentionallyCreatedSurplus-Summary.xlsx
+++ b/ICS/IntentionallyCreatedSurplus-Summary.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20354"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20361"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Rosenberg\Work\USU\Research\ColoradoRiver\RCode\ColoradoRiverFutures\ICS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7813440C-ABFB-4F68-9726-A64BD08D7559}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A24C01D3-FF84-4365-8D64-39C42A0071CF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="By User" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="42">
   <si>
     <t>Data Sources:</t>
   </si>
@@ -103,6 +104,54 @@
   </si>
   <si>
     <t>Year</t>
+  </si>
+  <si>
+    <t>Difference</t>
+  </si>
+  <si>
+    <t>Balance - Dec 2014 (AF)</t>
+  </si>
+  <si>
+    <t>Balance - Dec 2013 (AF)</t>
+  </si>
+  <si>
+    <t>Balance - Dec 2012 (AF)</t>
+  </si>
+  <si>
+    <t>Balance - Dec 2011 (AF)</t>
+  </si>
+  <si>
+    <t>Balance - Dec 2010 (AF)</t>
+  </si>
+  <si>
+    <t>User</t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>Balance</t>
+  </si>
+  <si>
+    <t>MWD</t>
+  </si>
+  <si>
+    <t>IID</t>
+  </si>
+  <si>
+    <t>SNWA</t>
+  </si>
+  <si>
+    <t>CAP</t>
+  </si>
+  <si>
+    <t>CRIT</t>
+  </si>
+  <si>
+    <t>GRIC</t>
+  </si>
+  <si>
+    <t>Balance - Dec 2019 (AF)</t>
   </si>
 </sst>
 </file>
@@ -179,7 +228,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
@@ -196,13 +245,18 @@
     <xf numFmtId="164" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -486,10 +540,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G25"/>
+  <dimension ref="A1:H31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -497,32 +551,33 @@
     <col min="1" max="1" width="30.7265625" customWidth="1"/>
     <col min="2" max="2" width="10" customWidth="1"/>
     <col min="3" max="3" width="11" customWidth="1"/>
-    <col min="4" max="4" width="9.81640625" customWidth="1"/>
+    <col min="4" max="4" width="10.54296875" customWidth="1"/>
     <col min="5" max="5" width="10.36328125" customWidth="1"/>
     <col min="6" max="6" width="9.08984375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>2</v>
       </c>
@@ -541,302 +596,1142 @@
       <c r="F6" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="G6" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
-        <v>23</v>
+        <v>41</v>
       </c>
       <c r="B7" s="2">
-        <v>343052</v>
+        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$F7,'By User'!$C$2:$C$43,Sheet1!B$6)</f>
+        <v>473504</v>
       </c>
       <c r="C7" s="2">
-        <v>698432</v>
+        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$F7,'By User'!$C$2:$C$43,Sheet1!C$6)</f>
+        <v>1053210</v>
       </c>
       <c r="D7" s="2">
-        <v>700448</v>
+        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$F7,'By User'!$C$2:$C$43,Sheet1!D$6)</f>
+        <v>785913</v>
       </c>
       <c r="E7" s="2">
         <f>SUM(B7:D7)</f>
-        <v>1741932</v>
-      </c>
-      <c r="F7" s="11">
-        <v>2018</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>7</v>
+        <v>2312627</v>
+      </c>
+      <c r="F7" s="15">
+        <v>2019</v>
+      </c>
+      <c r="G7" s="13">
+        <f>E7-E8</f>
+        <v>570695</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="5" t="s">
+        <v>23</v>
       </c>
       <c r="B8" s="2">
-        <v>126800</v>
+        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$F8,'By User'!$C$2:$C$43,Sheet1!B$6)</f>
+        <v>343052</v>
       </c>
       <c r="C8" s="2">
-        <v>552378</v>
+        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$F8,'By User'!$C$2:$C$43,Sheet1!C$6)</f>
+        <v>698432</v>
       </c>
       <c r="D8" s="2">
-        <v>582313</v>
+        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$F8,'By User'!$C$2:$C$43,Sheet1!D$6)</f>
+        <v>700448</v>
       </c>
       <c r="E8" s="2">
         <f>SUM(B8:D8)</f>
+        <v>1741932</v>
+      </c>
+      <c r="F8" s="10">
+        <v>2018</v>
+      </c>
+      <c r="G8" s="13">
+        <f>E8-E9</f>
+        <v>480441</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="2">
+        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$F9,'By User'!$C$2:$C$43,Sheet1!B$6)</f>
+        <v>126800</v>
+      </c>
+      <c r="C9" s="2">
+        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$F9,'By User'!$C$2:$C$43,Sheet1!C$6)</f>
+        <v>552378</v>
+      </c>
+      <c r="D9" s="2">
+        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$F9,'By User'!$C$2:$C$43,Sheet1!D$6)</f>
+        <v>582313</v>
+      </c>
+      <c r="E9" s="2">
+        <f>SUM(B9:D9)</f>
         <v>1261491</v>
       </c>
-      <c r="F8" s="12">
+      <c r="F9" s="11">
         <v>2017</v>
       </c>
-      <c r="G8" t="s">
+      <c r="G9" s="13">
+        <f t="shared" ref="G9:G15" si="0">E9-E10</f>
+        <v>511813</v>
+      </c>
+      <c r="H9" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="2">
+      <c r="B10" s="2">
+        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$F10,'By User'!$C$2:$C$43,Sheet1!B$6)</f>
         <v>103050</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C10" s="2">
+        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$F10,'By User'!$C$2:$C$43,Sheet1!C$6)</f>
         <v>115066</v>
       </c>
-      <c r="D9" s="2">
+      <c r="D10" s="2">
+        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$F10,'By User'!$C$2:$C$43,Sheet1!D$6)</f>
         <v>531562</v>
       </c>
-      <c r="E9" s="2">
-        <f t="shared" ref="E9:E10" si="0">SUM(B9:D9)</f>
+      <c r="E10" s="2">
+        <f t="shared" ref="E10:E16" si="1">SUM(B10:D10)</f>
         <v>749678</v>
       </c>
-      <c r="F9" s="12">
+      <c r="F10" s="11">
         <v>2016</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
+      <c r="G10" s="13">
+        <f t="shared" si="0"/>
+        <v>37814</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="2">
+      <c r="B11" s="2">
+        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$F11,'By User'!$C$2:$C$43,Sheet1!B$6)</f>
         <v>103050</v>
       </c>
-      <c r="C10" s="2">
+      <c r="C11" s="2">
+        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$F11,'By User'!$C$2:$C$43,Sheet1!C$6)</f>
         <v>97791</v>
       </c>
-      <c r="D10" s="2">
+      <c r="D11" s="2">
+        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$F11,'By User'!$C$2:$C$43,Sheet1!D$6)</f>
         <v>511023</v>
       </c>
-      <c r="E10" s="2">
+      <c r="E11" s="2">
+        <f t="shared" si="1"/>
+        <v>711864</v>
+      </c>
+      <c r="F11" s="11">
+        <v>2015</v>
+      </c>
+      <c r="G11" s="13">
         <f t="shared" si="0"/>
-        <v>711864</v>
-      </c>
-      <c r="F10" s="12">
-        <v>2015</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>8</v>
-      </c>
-      <c r="B11" s="2">
-        <v>100000</v>
-      </c>
-      <c r="C11" s="2">
-        <v>400000</v>
-      </c>
-      <c r="D11" s="2">
-        <v>125000</v>
-      </c>
-      <c r="E11" s="2">
-        <f t="shared" ref="E11:E13" si="1">SUM(B11:D11)</f>
-        <v>625000</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+        <v>-125036</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="B12" s="2">
-        <v>300000</v>
+        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$F12,'By User'!$C$2:$C$43,Sheet1!B$6)</f>
+        <v>103050</v>
       </c>
       <c r="C12" s="2">
-        <v>1500000</v>
+        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$F12,'By User'!$C$2:$C$43,Sheet1!C$6)</f>
+        <v>169085</v>
       </c>
       <c r="D12" s="2">
-        <v>300000</v>
+        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$F12,'By User'!$C$2:$C$43,Sheet1!D$6)</f>
+        <v>564765</v>
       </c>
       <c r="E12" s="2">
         <f t="shared" si="1"/>
-        <v>2100000</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+        <v>836900</v>
+      </c>
+      <c r="F12" s="11">
+        <v>2014</v>
+      </c>
+      <c r="G12" s="13">
+        <f t="shared" si="0"/>
+        <v>-281264</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="B13" s="2">
-        <v>300000</v>
+        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$F13,'By User'!$C$2:$C$43,Sheet1!B$6)</f>
+        <v>103050</v>
       </c>
       <c r="C13" s="2">
-        <v>400000</v>
+        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$F13,'By User'!$C$2:$C$43,Sheet1!C$6)</f>
+        <v>474063</v>
       </c>
       <c r="D13" s="2">
-        <v>300000</v>
+        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$F13,'By User'!$C$2:$C$43,Sheet1!D$6)</f>
+        <v>541051</v>
       </c>
       <c r="E13" s="2">
         <f t="shared" si="1"/>
+        <v>1118164</v>
+      </c>
+      <c r="F13" s="11">
+        <v>2013</v>
+      </c>
+      <c r="G13" s="13">
+        <f t="shared" si="0"/>
+        <v>-77476</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>29</v>
+      </c>
+      <c r="B14" s="2">
+        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$F14,'By User'!$C$2:$C$43,Sheet1!B$6)</f>
+        <v>103050</v>
+      </c>
+      <c r="C14" s="2">
+        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$F14,'By User'!$C$2:$C$43,Sheet1!C$6)</f>
+        <v>579786</v>
+      </c>
+      <c r="D14" s="2">
+        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$F14,'By User'!$C$2:$C$43,Sheet1!D$6)</f>
+        <v>512804</v>
+      </c>
+      <c r="E14" s="2">
+        <f t="shared" si="1"/>
+        <v>1195640</v>
+      </c>
+      <c r="F14" s="11">
+        <v>2012</v>
+      </c>
+      <c r="G14" s="13">
+        <f t="shared" si="0"/>
+        <v>169240</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15" s="2">
+        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$F15,'By User'!$C$2:$C$43,Sheet1!B$6)</f>
+        <v>103050</v>
+      </c>
+      <c r="C15" s="2">
+        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$F15,'By User'!$C$2:$C$43,Sheet1!C$6)</f>
+        <v>440678</v>
+      </c>
+      <c r="D15" s="2">
+        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$F15,'By User'!$C$2:$C$43,Sheet1!D$6)</f>
+        <v>482672</v>
+      </c>
+      <c r="E15" s="2">
+        <f t="shared" si="1"/>
+        <v>1026400</v>
+      </c>
+      <c r="F15" s="11">
+        <v>2011</v>
+      </c>
+      <c r="G15" s="13">
+        <f t="shared" si="0"/>
+        <v>211059</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>31</v>
+      </c>
+      <c r="B16" s="2">
+        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$F16,'By User'!$C$2:$C$43,Sheet1!B$6)</f>
+        <v>102094</v>
+      </c>
+      <c r="C16" s="2">
+        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$F16,'By User'!$C$2:$C$43,Sheet1!C$6)</f>
+        <v>261990</v>
+      </c>
+      <c r="D16" s="2">
+        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$F16,'By User'!$C$2:$C$43,Sheet1!D$6)</f>
+        <v>451257</v>
+      </c>
+      <c r="E16" s="2">
+        <f t="shared" si="1"/>
+        <v>815341</v>
+      </c>
+      <c r="F16" s="11">
+        <v>2010</v>
+      </c>
+      <c r="G16" s="13"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>8</v>
+      </c>
+      <c r="B17" s="2">
+        <v>100000</v>
+      </c>
+      <c r="C17" s="2">
+        <v>400000</v>
+      </c>
+      <c r="D17" s="2">
+        <v>125000</v>
+      </c>
+      <c r="E17" s="2">
+        <f t="shared" ref="E17:E19" si="2">SUM(B17:D17)</f>
+        <v>625000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>9</v>
+      </c>
+      <c r="B18" s="2">
+        <v>300000</v>
+      </c>
+      <c r="C18" s="2">
+        <v>1500000</v>
+      </c>
+      <c r="D18" s="2">
+        <v>300000</v>
+      </c>
+      <c r="E18" s="2">
+        <f t="shared" si="2"/>
+        <v>2100000</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>10</v>
+      </c>
+      <c r="B19" s="2">
+        <v>300000</v>
+      </c>
+      <c r="C19" s="2">
+        <v>400000</v>
+      </c>
+      <c r="D19" s="2">
+        <v>300000</v>
+      </c>
+      <c r="E19" s="2">
+        <f t="shared" si="2"/>
         <v>1000000</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
         <v>20</v>
       </c>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A16" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="B16" s="9" t="str">
-        <f>B6</f>
-        <v>Arizona</v>
-      </c>
-      <c r="C16" s="9" t="str">
-        <f t="shared" ref="C16:E16" si="2">C6</f>
-        <v>California</v>
-      </c>
-      <c r="D16" s="9" t="str">
-        <f t="shared" si="2"/>
-        <v>Nevada</v>
-      </c>
-      <c r="E16" s="9" t="str">
-        <f t="shared" si="2"/>
-        <v>Total</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A17" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B17" s="7">
-        <v>100000</v>
-      </c>
-      <c r="C17" s="7">
-        <v>400000</v>
-      </c>
-      <c r="D17" s="7">
-        <v>125000</v>
-      </c>
-      <c r="E17" s="7">
-        <f t="shared" ref="E17:E19" si="3">SUM(B17:D17)</f>
-        <v>625000</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A18" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="B18" s="7">
-        <v>500000</v>
-      </c>
-      <c r="C18" s="7">
-        <v>1700000</v>
-      </c>
-      <c r="D18" s="7">
-        <v>500000</v>
-      </c>
-      <c r="E18" s="7">
-        <f t="shared" si="3"/>
-        <v>2700000</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A19" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B19" s="7">
-        <f>B13</f>
-        <v>300000</v>
-      </c>
-      <c r="C19" s="7">
-        <f t="shared" ref="C19:D19" si="4">C13</f>
-        <v>400000</v>
-      </c>
-      <c r="D19" s="7">
-        <f t="shared" si="4"/>
-        <v>300000</v>
-      </c>
-      <c r="E19" s="7">
-        <f t="shared" si="3"/>
-        <v>1000000</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A20" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="B20" s="10"/>
-      <c r="C20" s="10"/>
-      <c r="D20" s="10"/>
-      <c r="E20" s="10"/>
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A21" t="s">
-        <v>19</v>
-      </c>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
+      <c r="A22" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B22" s="9" t="str">
+        <f>B6</f>
+        <v>Arizona</v>
+      </c>
+      <c r="C22" s="9" t="str">
+        <f t="shared" ref="C22:E22" si="3">C6</f>
+        <v>California</v>
+      </c>
+      <c r="D22" s="9" t="str">
+        <f t="shared" si="3"/>
+        <v>Nevada</v>
+      </c>
+      <c r="E22" s="9" t="str">
+        <f t="shared" si="3"/>
+        <v>Total</v>
+      </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A23" s="1" t="s">
+      <c r="A23" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B23" s="7">
+        <v>100000</v>
+      </c>
+      <c r="C23" s="7">
+        <v>400000</v>
+      </c>
+      <c r="D23" s="7">
+        <v>125000</v>
+      </c>
+      <c r="E23" s="7">
+        <f t="shared" ref="E23:E25" si="4">SUM(B23:D23)</f>
+        <v>625000</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A24" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B24" s="7">
+        <v>500000</v>
+      </c>
+      <c r="C24" s="7">
+        <v>1700000</v>
+      </c>
+      <c r="D24" s="7">
+        <v>500000</v>
+      </c>
+      <c r="E24" s="7">
+        <f t="shared" si="4"/>
+        <v>2700000</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A25" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B25" s="7">
+        <f>B19</f>
+        <v>300000</v>
+      </c>
+      <c r="C25" s="7">
+        <f t="shared" ref="C25:D25" si="5">C19</f>
+        <v>400000</v>
+      </c>
+      <c r="D25" s="7">
+        <f t="shared" si="5"/>
+        <v>300000</v>
+      </c>
+      <c r="E25" s="7">
+        <f t="shared" si="4"/>
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A26" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B26" s="12"/>
+      <c r="C26" s="12"/>
+      <c r="D26" s="12"/>
+      <c r="E26" s="12"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>19</v>
+      </c>
+      <c r="B27" s="2"/>
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B28" s="2"/>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A29" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A24" t="s">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
         <v>11</v>
       </c>
-      <c r="B24" s="4">
+      <c r="B30" s="4">
         <v>0.05</v>
       </c>
-      <c r="C24" s="4">
+      <c r="C30" s="4">
         <v>0.05</v>
       </c>
-      <c r="D24" s="4">
+      <c r="D30" s="4">
         <v>0.05</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A25" t="s">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
         <v>17</v>
       </c>
-      <c r="B25" s="4">
+      <c r="B31" s="4">
         <v>0.03</v>
       </c>
-      <c r="C25" s="4">
+      <c r="C31" s="4">
         <v>0.03</v>
       </c>
-      <c r="D25" s="4">
+      <c r="D31" s="4">
         <v>0.03</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A20:E20"/>
+    <mergeCell ref="A26:E26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46D265CD-11FF-4B0E-A32F-7305DFCA8DC1}">
+  <dimension ref="A1:H43"/>
+  <sheetViews>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="4" max="4" width="11.08984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>2011</v>
+      </c>
+      <c r="B2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="2">
+        <f>100000+3050</f>
+        <v>103050</v>
+      </c>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>2011</v>
+      </c>
+      <c r="B3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="2">
+        <f>344439+66000+24397</f>
+        <v>434836</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>2011</v>
+      </c>
+      <c r="B4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="2">
+        <f>5842</f>
+        <v>5842</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>2011</v>
+      </c>
+      <c r="B5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="2">
+        <f>47523+28395+3704+400000+3050</f>
+        <v>482672</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>2010</v>
+      </c>
+      <c r="B6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6" s="2">
+        <f>100000+2094</f>
+        <v>102094</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>2010</v>
+      </c>
+      <c r="B7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="2">
+        <f>173217+66000+16750</f>
+        <v>255967</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>2010</v>
+      </c>
+      <c r="B8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" s="2">
+        <v>6023</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>2010</v>
+      </c>
+      <c r="B9" t="s">
+        <v>37</v>
+      </c>
+      <c r="C9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" s="2">
+        <f>19798+28566+799+400000+2094</f>
+        <v>451257</v>
+      </c>
+      <c r="F9" s="14"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>2012</v>
+      </c>
+      <c r="B10" t="s">
+        <v>38</v>
+      </c>
+      <c r="C10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D10" s="2">
+        <f>100000+3050</f>
+        <v>103050</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>2012</v>
+      </c>
+      <c r="B11" t="s">
+        <v>35</v>
+      </c>
+      <c r="C11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" s="2">
+        <f>489389+66000+24397</f>
+        <v>579786</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>2012</v>
+      </c>
+      <c r="B12" t="s">
+        <v>36</v>
+      </c>
+      <c r="C12" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A13">
+        <v>2012</v>
+      </c>
+      <c r="B13" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13" s="2">
+        <f>77162+29870+2722+400000+3050</f>
+        <v>512804</v>
+      </c>
+      <c r="E13" s="14"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A14">
+        <v>2013</v>
+      </c>
+      <c r="B14" t="s">
+        <v>38</v>
+      </c>
+      <c r="C14" t="s">
+        <v>3</v>
+      </c>
+      <c r="D14" s="2">
+        <f>100000+3050</f>
+        <v>103050</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A15">
+        <v>2013</v>
+      </c>
+      <c r="B15" t="s">
+        <v>35</v>
+      </c>
+      <c r="C15" t="s">
+        <v>4</v>
+      </c>
+      <c r="D15" s="2">
+        <f>383666+66000+24397</f>
+        <v>474063</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A16">
+        <v>2013</v>
+      </c>
+      <c r="B16" t="s">
+        <v>36</v>
+      </c>
+      <c r="C16" t="s">
+        <v>4</v>
+      </c>
+      <c r="D16" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A17">
+        <v>2013</v>
+      </c>
+      <c r="B17" t="s">
+        <v>37</v>
+      </c>
+      <c r="C17" t="s">
+        <v>5</v>
+      </c>
+      <c r="D17" s="2">
+        <f>106461+29925+1615+400000+3050</f>
+        <v>541051</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A18">
+        <v>2014</v>
+      </c>
+      <c r="B18" t="s">
+        <v>38</v>
+      </c>
+      <c r="C18" t="s">
+        <v>3</v>
+      </c>
+      <c r="D18" s="2">
+        <f>100000+3050</f>
+        <v>103050</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A19">
+        <v>2014</v>
+      </c>
+      <c r="B19" t="s">
+        <v>35</v>
+      </c>
+      <c r="C19" t="s">
+        <v>4</v>
+      </c>
+      <c r="D19" s="2">
+        <f>61764+65000+24397</f>
+        <v>151161</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A20">
+        <v>2014</v>
+      </c>
+      <c r="B20" t="s">
+        <v>36</v>
+      </c>
+      <c r="C20" t="s">
+        <v>4</v>
+      </c>
+      <c r="D20" s="2">
+        <v>17924</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A21">
+        <v>2014</v>
+      </c>
+      <c r="B21" t="s">
+        <v>37</v>
+      </c>
+      <c r="C21" t="s">
+        <v>5</v>
+      </c>
+      <c r="D21" s="2">
+        <v>564765</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A22">
+        <v>2015</v>
+      </c>
+      <c r="B22" t="s">
+        <v>38</v>
+      </c>
+      <c r="C22" t="s">
+        <v>3</v>
+      </c>
+      <c r="D22" s="2">
+        <f>100000+3050</f>
+        <v>103050</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A23">
+        <v>2015</v>
+      </c>
+      <c r="B23" t="s">
+        <v>35</v>
+      </c>
+      <c r="C23" t="s">
+        <v>4</v>
+      </c>
+      <c r="D23" s="2">
+        <f>56008+24397</f>
+        <v>80405</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A24">
+        <v>2015</v>
+      </c>
+      <c r="B24" t="s">
+        <v>36</v>
+      </c>
+      <c r="C24" t="s">
+        <v>4</v>
+      </c>
+      <c r="D24" s="2">
+        <v>17386</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A25">
+        <v>2015</v>
+      </c>
+      <c r="B25" t="s">
+        <v>37</v>
+      </c>
+      <c r="C25" t="s">
+        <v>5</v>
+      </c>
+      <c r="D25" s="2">
+        <v>511023</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A26">
+        <v>2016</v>
+      </c>
+      <c r="B26" t="s">
+        <v>38</v>
+      </c>
+      <c r="C26" t="s">
+        <v>3</v>
+      </c>
+      <c r="D26" s="2">
+        <f>100000+3050</f>
+        <v>103050</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A27">
+        <v>2016</v>
+      </c>
+      <c r="B27" t="s">
+        <v>35</v>
+      </c>
+      <c r="C27" t="s">
+        <v>4</v>
+      </c>
+      <c r="D27" s="2">
+        <f>4644+56008+24397</f>
+        <v>85049</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A28">
+        <v>2016</v>
+      </c>
+      <c r="B28" t="s">
+        <v>36</v>
+      </c>
+      <c r="C28" t="s">
+        <v>4</v>
+      </c>
+      <c r="D28" s="2">
+        <v>30017</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A29">
+        <v>2016</v>
+      </c>
+      <c r="B29" t="s">
+        <v>37</v>
+      </c>
+      <c r="C29" t="s">
+        <v>5</v>
+      </c>
+      <c r="D29" s="2">
+        <v>531562</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A30">
+        <v>2017</v>
+      </c>
+      <c r="B30" t="s">
+        <v>38</v>
+      </c>
+      <c r="C30" t="s">
+        <v>3</v>
+      </c>
+      <c r="D30" s="2">
+        <v>126800</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A31">
+        <v>2017</v>
+      </c>
+      <c r="B31" t="s">
+        <v>35</v>
+      </c>
+      <c r="C31" t="s">
+        <v>4</v>
+      </c>
+      <c r="D31" s="2">
+        <v>478628</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A32">
+        <v>2017</v>
+      </c>
+      <c r="B32" t="s">
+        <v>36</v>
+      </c>
+      <c r="C32" t="s">
+        <v>4</v>
+      </c>
+      <c r="D32" s="2">
+        <v>73750</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A33">
+        <v>2017</v>
+      </c>
+      <c r="B33" t="s">
+        <v>37</v>
+      </c>
+      <c r="C33" t="s">
+        <v>5</v>
+      </c>
+      <c r="D33" s="2">
+        <v>582313</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A34">
+        <v>2018</v>
+      </c>
+      <c r="B34" t="s">
+        <v>38</v>
+      </c>
+      <c r="C34" t="s">
+        <v>3</v>
+      </c>
+      <c r="D34" s="2">
+        <v>343052</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A35">
+        <v>2018</v>
+      </c>
+      <c r="B35" t="s">
+        <v>35</v>
+      </c>
+      <c r="C35" t="s">
+        <v>4</v>
+      </c>
+      <c r="D35" s="2">
+        <v>624682</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A36">
+        <v>2018</v>
+      </c>
+      <c r="B36" t="s">
+        <v>36</v>
+      </c>
+      <c r="C36" t="s">
+        <v>4</v>
+      </c>
+      <c r="D36" s="2">
+        <v>73750</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A37">
+        <v>2018</v>
+      </c>
+      <c r="B37" t="s">
+        <v>37</v>
+      </c>
+      <c r="C37" t="s">
+        <v>5</v>
+      </c>
+      <c r="D37" s="2">
+        <v>700448</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A38">
+        <v>2019</v>
+      </c>
+      <c r="B38" t="s">
+        <v>38</v>
+      </c>
+      <c r="C38" t="s">
+        <v>3</v>
+      </c>
+      <c r="D38" s="2">
+        <v>362557</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A39">
+        <v>2019</v>
+      </c>
+      <c r="B39" t="s">
+        <v>39</v>
+      </c>
+      <c r="C39" t="s">
+        <v>3</v>
+      </c>
+      <c r="D39" s="2">
+        <v>5647</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A40">
+        <v>2019</v>
+      </c>
+      <c r="B40" t="s">
+        <v>40</v>
+      </c>
+      <c r="C40" t="s">
+        <v>3</v>
+      </c>
+      <c r="D40" s="2">
+        <v>105300</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A41">
+        <v>2019</v>
+      </c>
+      <c r="B41" t="s">
+        <v>35</v>
+      </c>
+      <c r="C41" t="s">
+        <v>4</v>
+      </c>
+      <c r="D41" s="2">
+        <v>979460</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A42">
+        <v>2019</v>
+      </c>
+      <c r="B42" t="s">
+        <v>36</v>
+      </c>
+      <c r="C42" t="s">
+        <v>4</v>
+      </c>
+      <c r="D42" s="2">
+        <v>73750</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A43">
+        <v>2019</v>
+      </c>
+      <c r="B43" t="s">
+        <v>37</v>
+      </c>
+      <c r="C43" t="s">
+        <v>5</v>
+      </c>
+      <c r="D43" s="2">
+        <v>785913</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>